<commit_message>
fix: update end date for Plutonchefskurs 2 in events.csv
</commit_message>
<xml_diff>
--- a/public/events.xlsx
+++ b/public/events.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="171">
   <si>
     <t xml:space="preserve">KURSKOD</t>
   </si>
@@ -220,7 +220,7 @@
     <t xml:space="preserve">2026-11-03, 2027-02-05</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-11-08, 2027-02-27</t>
+    <t xml:space="preserve">2026-11-08, 2027-02-07</t>
   </si>
   <si>
     <t xml:space="preserve">BLG</t>
@@ -248,9 +248,6 @@
   </si>
   <si>
     <t xml:space="preserve">Kvarn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2026-11-08, 2027-02-07</t>
   </si>
   <si>
     <t xml:space="preserve">MAHFK2011231</t>
@@ -793,13 +790,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -845,7 +842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -872,7 +869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -899,7 +896,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -926,7 +923,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -953,7 +950,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -980,7 +977,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1007,7 +1004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1034,7 +1031,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1058,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1088,7 +1085,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1115,7 +1112,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1142,7 +1139,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1169,7 +1166,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1196,7 +1193,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1223,7 +1220,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1250,7 +1247,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1277,7 +1274,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1304,7 +1301,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1331,7 +1328,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
@@ -1358,7 +1355,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -1385,7 +1382,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -1412,7 +1409,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
@@ -1439,7 +1436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1466,7 +1463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -1493,7 +1490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -1520,7 +1517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -1547,7 +1544,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
@@ -1574,7 +1571,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>49</v>
       </c>
@@ -1601,7 +1598,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -1628,7 +1625,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>51</v>
       </c>
@@ -1655,7 +1652,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
@@ -1682,7 +1679,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
@@ -1709,7 +1706,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
@@ -1739,7 +1736,7 @@
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>55</v>
       </c>
@@ -1769,7 +1766,7 @@
       </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>61</v>
       </c>
@@ -1799,7 +1796,7 @@
       </c>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -1830,7 +1827,7 @@
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
@@ -1860,7 +1857,7 @@
       </c>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>68</v>
       </c>
@@ -1890,7 +1887,7 @@
       </c>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
@@ -1920,7 +1917,7 @@
       </c>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
@@ -1951,7 +1948,7 @@
       </c>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
@@ -1962,7 +1959,7 @@
         <v>64</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E42" s="2" t="n">
         <v>46264</v>
@@ -1981,12 +1978,12 @@
       </c>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>46479</v>
@@ -2011,7 +2008,7 @@
       </c>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -2019,10 +2016,10 @@
         <v>23</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="E44" s="2" t="n">
         <v>46068</v>
@@ -2040,12 +2037,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C45" s="2" t="n">
         <v>46080</v>
@@ -2070,12 +2067,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C46" s="2" t="n">
         <v>46080</v>
@@ -2099,12 +2096,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C47" s="2" t="n">
         <v>46157</v>
@@ -2128,12 +2125,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C48" s="2" t="n">
         <v>46185</v>
@@ -2158,12 +2155,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C49" s="2" t="n">
         <v>46262</v>
@@ -2187,12 +2184,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C50" s="2" t="n">
         <v>46332</v>
@@ -2218,10 +2215,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="C51" s="2" t="n">
         <v>46086</v>
@@ -2245,12 +2242,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="C52" s="2" t="n">
         <v>46087</v>
@@ -2274,12 +2271,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="C53" s="2" t="n">
         <v>46104</v>
@@ -2303,12 +2300,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="C54" s="2" t="n">
         <v>46114</v>
@@ -2332,12 +2329,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C55" s="2" t="n">
         <v>46104</v>
@@ -2361,12 +2358,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C56" s="2" t="n">
         <v>46114</v>
@@ -2390,12 +2387,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C57" s="2" t="n">
         <v>46155</v>
@@ -2420,12 +2417,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C58" s="2" t="n">
         <v>46351</v>
@@ -2450,12 +2447,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="C59" s="2" t="n">
         <v>46167</v>
@@ -2479,12 +2476,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C60" s="2" t="n">
         <v>46174</v>
@@ -2508,12 +2505,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>46200</v>
@@ -2526,21 +2523,21 @@
         <v>46103</v>
       </c>
       <c r="F61" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C62" s="2" t="n">
         <v>46099</v>
@@ -2553,21 +2550,21 @@
         <v>46033</v>
       </c>
       <c r="F62" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="C63" s="2" t="n">
         <v>46099</v>
@@ -2580,21 +2577,21 @@
         <v>46033</v>
       </c>
       <c r="F63" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>46097</v>
@@ -2607,21 +2604,21 @@
         <v>46033</v>
       </c>
       <c r="F64" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G64" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="H64" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C65" s="2" t="n">
         <v>46202</v>
@@ -2634,21 +2631,21 @@
         <v>46103</v>
       </c>
       <c r="F65" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="H65" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C66" s="2" t="n">
         <v>46202</v>
@@ -2661,21 +2658,21 @@
         <v>46103</v>
       </c>
       <c r="F66" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G66" s="1" t="s">
+      <c r="H66" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="C67" s="2" t="n">
         <v>46314</v>
@@ -2689,21 +2686,21 @@
         <v>46241</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G67" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="H67" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C68" s="2" t="n">
         <v>46314</v>
@@ -2717,21 +2714,21 @@
         <v>46241</v>
       </c>
       <c r="F68" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G68" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="H68" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C69" s="2" t="n">
         <v>46090</v>
@@ -2744,21 +2741,21 @@
         <v>46033</v>
       </c>
       <c r="F69" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G69" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G69" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="H69" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="C70" s="2" t="n">
         <v>46091</v>
@@ -2771,21 +2768,21 @@
         <v>46033</v>
       </c>
       <c r="F70" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G70" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="C71" s="2" t="n">
         <v>46091</v>
@@ -2798,16 +2795,16 @@
         <v>46033</v>
       </c>
       <c r="F71" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>61</v>
       </c>
@@ -2825,21 +2822,21 @@
         <v>45984</v>
       </c>
       <c r="F72" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C73" s="2" t="n">
         <v>46069</v>
@@ -2852,21 +2849,21 @@
         <v>45984</v>
       </c>
       <c r="F73" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G73" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="C74" s="2" t="n">
         <v>46073</v>
@@ -2879,16 +2876,16 @@
         <v>45984</v>
       </c>
       <c r="F74" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>30</v>
       </c>
@@ -2906,16 +2903,16 @@
         <v>45998</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>22</v>
       </c>
@@ -2933,16 +2930,16 @@
         <v>45998</v>
       </c>
       <c r="F76" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>24</v>
       </c>
@@ -2960,16 +2957,16 @@
         <v>46026</v>
       </c>
       <c r="F77" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>68</v>
       </c>
@@ -2987,16 +2984,16 @@
         <v>46166</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>26</v>
       </c>
@@ -3014,16 +3011,16 @@
         <v>46243</v>
       </c>
       <c r="F79" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
         <v>32</v>
       </c>
@@ -3041,21 +3038,21 @@
         <v>46243</v>
       </c>
       <c r="F80" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G80" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="C81" s="2" t="n">
         <v>46146</v>
@@ -3067,21 +3064,21 @@
         <v>46061</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G81" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H81" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C82" s="2" t="n">
         <v>46085</v>
@@ -3094,21 +3091,21 @@
         <v>45998</v>
       </c>
       <c r="F82" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G82" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="H82" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C83" s="2" t="n">
         <v>46169</v>
@@ -3121,21 +3118,21 @@
         <v>46082</v>
       </c>
       <c r="F83" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G83" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="H83" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C84" s="2" t="n">
         <v>46288</v>
@@ -3148,21 +3145,21 @@
         <v>46201</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C85" s="2" t="n">
         <v>46344</v>
@@ -3175,21 +3172,21 @@
         <v>46257</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C86" s="2" t="n">
         <v>46078</v>
@@ -3202,21 +3199,21 @@
         <v>45991</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C87" s="2" t="n">
         <v>46083</v>
@@ -3229,10 +3226,10 @@
         <v>45998</v>
       </c>
       <c r="F87" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>36</v>
@@ -3240,10 +3237,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C88" s="2" t="n">
         <v>46085</v>
@@ -3256,47 +3253,47 @@
         <v>45998</v>
       </c>
       <c r="F88" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C89" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="D89" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="E89" s="2" t="n">
         <v>46103</v>
       </c>
       <c r="F89" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G89" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="C90" s="2" t="n">
         <v>46253</v>
@@ -3309,21 +3306,21 @@
         <v>46166</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="C91" s="2" t="n">
         <v>46253</v>
@@ -3335,21 +3332,21 @@
         <v>46166</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C92" s="2" t="n">
         <v>46251</v>
@@ -3362,16 +3359,16 @@
         <v>46166</v>
       </c>
       <c r="F92" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G92" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>55</v>
       </c>
@@ -3388,17 +3385,17 @@
         <v>46089</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>55</v>
       </c>
@@ -3415,17 +3412,17 @@
         <v>46089</v>
       </c>
       <c r="F94" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G94" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>55</v>
       </c>
@@ -3442,7 +3439,7 @@
         <v>46152</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>13</v>
@@ -3452,7 +3449,7 @@
       </c>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>55</v>
       </c>
@@ -3469,17 +3466,17 @@
         <v>46180</v>
       </c>
       <c r="F96" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G96" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>55</v>
       </c>
@@ -3496,17 +3493,17 @@
         <v>46310</v>
       </c>
       <c r="F97" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G97" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>24</v>
       </c>
@@ -3523,17 +3520,17 @@
         <v>46278</v>
       </c>
       <c r="F98" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G98" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>61</v>
       </c>
@@ -3550,7 +3547,7 @@
         <v>46152</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>13</v>
@@ -3560,7 +3557,7 @@
       </c>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>61</v>
       </c>
@@ -3577,17 +3574,17 @@
         <v>46278</v>
       </c>
       <c r="F100" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G100" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J100" s="2"/>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>61</v>
       </c>
@@ -3604,17 +3601,17 @@
         <v>46307</v>
       </c>
       <c r="F101" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G101" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J101" s="2"/>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>32</v>
       </c>
@@ -3631,17 +3628,17 @@
         <v>46307</v>
       </c>
       <c r="F102" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G102" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J102" s="2"/>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
         <v>26</v>
       </c>
@@ -3658,22 +3655,22 @@
         <v>46307</v>
       </c>
       <c r="F103" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G103" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J103" s="2"/>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C104" s="2" t="n">
         <v>46293</v>
@@ -3685,22 +3682,22 @@
         <v>46180</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G104" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J104" s="2"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="H104" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J104" s="2"/>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="C105" s="2" t="n">
         <v>46293</v>
@@ -3712,22 +3709,22 @@
         <v>46180</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J105" s="2"/>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C106" s="2" t="n">
         <v>46135</v>
@@ -3739,22 +3736,22 @@
         <v>46113</v>
       </c>
       <c r="F106" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G106" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G106" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H106" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J106" s="2"/>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C107" s="2" t="n">
         <v>46135</v>
@@ -3766,22 +3763,22 @@
         <v>46113</v>
       </c>
       <c r="F107" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G107" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G107" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H107" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J107" s="2"/>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C108" s="2" t="n">
         <v>46247</v>
@@ -3793,22 +3790,22 @@
         <v>46180</v>
       </c>
       <c r="F108" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G108" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G108" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J108" s="2"/>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C109" s="2" t="n">
         <v>46268</v>
@@ -3820,22 +3817,22 @@
         <v>46236</v>
       </c>
       <c r="F109" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G109" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G109" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="H109" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J109" s="2"/>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C110" s="2" t="n">
         <v>46338</v>
@@ -3847,22 +3844,22 @@
         <v>46299</v>
       </c>
       <c r="F110" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G110" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G110" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="H110" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J110" s="2"/>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C111" s="2" t="n">
         <v>46169</v>
@@ -3874,22 +3871,22 @@
         <v>46131</v>
       </c>
       <c r="F111" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G111" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="H111" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J111" s="2"/>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C112" s="2" t="n">
         <v>46309</v>
@@ -3901,22 +3898,22 @@
         <v>46271</v>
       </c>
       <c r="F112" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G112" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G112" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="H112" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J112" s="2"/>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C113" s="2" t="n">
         <v>46042</v>
@@ -3928,7 +3925,7 @@
         <v>45976</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>13</v>
@@ -3938,12 +3935,12 @@
       </c>
       <c r="J113" s="2"/>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C114" s="2" t="n">
         <v>46069</v>
@@ -3955,22 +3952,22 @@
         <v>46040</v>
       </c>
       <c r="F114" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G114" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J114" s="2"/>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="C115" s="2" t="n">
         <v>46069</v>
@@ -3982,22 +3979,22 @@
         <v>46040</v>
       </c>
       <c r="F115" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J115" s="2"/>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C116" s="2" t="n">
         <v>46076</v>
@@ -4009,22 +4006,22 @@
         <v>46041</v>
       </c>
       <c r="F116" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G116" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J116" s="2"/>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C117" s="2" t="n">
         <v>46251</v>
@@ -4036,61 +4033,61 @@
         <v>46180</v>
       </c>
       <c r="F117" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G117" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J117" s="2"/>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B118" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="C118" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D118" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="E118" s="2" t="n">
         <v>46054</v>
       </c>
       <c r="F118" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G118" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J118" s="2"/>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="C119" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="D119" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="E119" s="2" t="n">
         <v>46257</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>13</v>
@@ -4100,12 +4097,12 @@
       </c>
       <c r="J119" s="2"/>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="C120" s="2" t="n">
         <v>46328</v>
@@ -4117,22 +4114,22 @@
         <v>46271</v>
       </c>
       <c r="F120" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G120" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J120" s="2"/>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="C121" s="2" t="n">
         <v>46339</v>
@@ -4144,22 +4141,22 @@
         <v>46310</v>
       </c>
       <c r="F121" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J121" s="2"/>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C122" s="2" t="n">
         <v>46129</v>
@@ -4171,22 +4168,22 @@
         <v>46113</v>
       </c>
       <c r="F122" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G122" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J122" s="2"/>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C123" s="2" t="n">
         <v>46339</v>
@@ -4198,22 +4195,22 @@
         <v>46310</v>
       </c>
       <c r="F123" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G123" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J123" s="2"/>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C124" s="2" t="n">
         <v>46137</v>
@@ -4225,7 +4222,7 @@
         <v>46103</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>13</v>
@@ -4234,15 +4231,15 @@
         <v>36</v>
       </c>
       <c r="J124" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C125" s="2" t="n">
         <v>46314</v>
@@ -4254,7 +4251,7 @@
         <v>46285</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>13</v>
@@ -4264,12 +4261,12 @@
       </c>
       <c r="J125" s="2"/>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="C126" s="2" t="n">
         <v>46342</v>
@@ -4281,25 +4278,18 @@
         <v>46306</v>
       </c>
       <c r="F126" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G126" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G126" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="H126" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J126" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J126">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="UND525SFS47"/>
-        <filter val="UNDGK311SF11"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J126"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Update course events and templates with new last modified dates and course codes
- Changed lastModified dates for multiple course events in hemvarn_course_events.json to "20260109-170517".
- Updated course code for "Gk Tung släpkärra" in hemvarn_course_templates_enriched.json to "LOGGK8481089".
- Modified event details in events.csv for "GK MRPAS" to reflect new dates and location.
- Adjusted create_templates.py to align with updated course code for "Gk Tung släpkärra".
</commit_message>
<xml_diff>
--- a/public/events.xlsx
+++ b/public/events.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$126</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$125</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="171">
   <si>
     <t xml:space="preserve">KURSKOD</t>
   </si>
@@ -793,10 +793,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J126"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F108" activeCellId="0" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2642,37 +2642,38 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>46202</v>
+        <v>46314</v>
       </c>
       <c r="D66" s="2" t="n">
-        <f aca="false">C66+6</f>
-        <v>46208</v>
+        <f aca="false">C66+4</f>
+        <v>46318</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>46103</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>107</v>
+        <f aca="false">C66-73</f>
+        <v>46241</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C67" s="2" t="n">
         <v>46314</v>
@@ -2692,7 +2693,7 @@
         <v>98</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2703,17 +2704,16 @@
         <v>90</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>46314</v>
+        <v>46090</v>
       </c>
       <c r="D68" s="2" t="n">
         <f aca="false">C68+4</f>
-        <v>46318</v>
+        <v>46094</v>
       </c>
       <c r="E68" s="2" t="n">
-        <f aca="false">C68-73</f>
-        <v>46241</v>
-      </c>
-      <c r="F68" s="2" t="s">
+        <v>46033</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>97</v>
       </c>
       <c r="G68" s="1" t="s">
@@ -2725,37 +2725,37 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="C69" s="2" t="n">
-        <v>46090</v>
+        <v>46091</v>
       </c>
       <c r="D69" s="2" t="n">
         <f aca="false">C69+4</f>
-        <v>46094</v>
+        <v>46095</v>
       </c>
       <c r="E69" s="2" t="n">
         <v>46033</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>97</v>
+      <c r="F69" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C70" s="2" t="n">
         <v>46091</v>
@@ -2767,7 +2767,7 @@
       <c r="E70" s="2" t="n">
         <v>46033</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F70" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G70" s="1" t="s">
@@ -2779,53 +2779,53 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>115</v>
+        <v>62</v>
       </c>
       <c r="C71" s="2" t="n">
-        <v>46091</v>
+        <v>46038</v>
       </c>
       <c r="D71" s="2" t="n">
-        <f aca="false">C71+4</f>
-        <v>46095</v>
+        <f aca="false">C71+9</f>
+        <v>46047</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>46033</v>
+        <v>45984</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>62</v>
+        <v>118</v>
       </c>
       <c r="C72" s="2" t="n">
-        <v>46038</v>
+        <v>46069</v>
       </c>
       <c r="D72" s="2" t="n">
-        <f aca="false">C72+9</f>
-        <v>46047</v>
+        <f aca="false">C72+13</f>
+        <v>46082</v>
       </c>
       <c r="E72" s="2" t="n">
         <v>45984</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>19</v>
@@ -2833,26 +2833,26 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C73" s="2" t="n">
-        <v>46069</v>
+        <v>46073</v>
       </c>
       <c r="D73" s="2" t="n">
-        <f aca="false">C73+13</f>
+        <f aca="false">C73+9</f>
         <v>46082</v>
       </c>
       <c r="E73" s="2" t="n">
         <v>45984</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>19</v>
@@ -2860,23 +2860,23 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="C74" s="2" t="n">
-        <v>46073</v>
+        <v>46083</v>
       </c>
       <c r="D74" s="2" t="n">
-        <f aca="false">C74+9</f>
-        <v>46082</v>
+        <f aca="false">C74+4</f>
+        <v>46087</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>45984</v>
+        <v>45998</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>122</v>
@@ -2887,23 +2887,23 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C75" s="2" t="n">
-        <v>46083</v>
+        <v>46085</v>
       </c>
       <c r="D75" s="2" t="n">
         <f aca="false">C75+4</f>
-        <v>46087</v>
+        <v>46089</v>
       </c>
       <c r="E75" s="2" t="n">
         <v>45998</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>122</v>
@@ -2914,26 +2914,26 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C76" s="2" t="n">
-        <v>46085</v>
+        <v>46097</v>
       </c>
       <c r="D76" s="2" t="n">
-        <f aca="false">C76+4</f>
-        <v>46089</v>
+        <f aca="false">C76+9</f>
+        <v>46106</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>45998</v>
+        <v>46026</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>19</v>
@@ -2941,26 +2941,26 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="C77" s="2" t="n">
-        <v>46097</v>
+        <v>46251</v>
       </c>
       <c r="D77" s="2" t="n">
-        <f aca="false">C77+9</f>
-        <v>46106</v>
+        <f aca="false">C77+4</f>
+        <v>46255</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>46026</v>
+        <v>46166</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>19</v>
@@ -2968,37 +2968,37 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C78" s="2" t="n">
-        <v>46251</v>
+        <v>46328</v>
       </c>
       <c r="D78" s="2" t="n">
-        <f aca="false">C78+4</f>
-        <v>46255</v>
+        <f aca="false">C78+9</f>
+        <v>46337</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>46166</v>
+        <v>46243</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>26</v>
+      <c r="A79" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C79" s="2" t="n">
         <v>46328</v>
@@ -3021,53 +3021,53 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="6" t="s">
-        <v>32</v>
+      <c r="A80" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="C80" s="2" t="n">
-        <v>46328</v>
+        <v>46146</v>
       </c>
       <c r="D80" s="2" t="n">
-        <f aca="false">C80+9</f>
-        <v>46337</v>
+        <v>46146</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>46243</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>126</v>
+        <v>46061</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C81" s="2" t="n">
-        <v>46146</v>
+        <v>46085</v>
       </c>
       <c r="D81" s="2" t="n">
-        <v>46146</v>
+        <f aca="false">C81+4</f>
+        <v>46089</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>46061</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>123</v>
+        <v>45998</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>14</v>
@@ -3081,14 +3081,14 @@
         <v>132</v>
       </c>
       <c r="C82" s="2" t="n">
-        <v>46085</v>
+        <v>46169</v>
       </c>
       <c r="D82" s="2" t="n">
         <f aca="false">C82+4</f>
-        <v>46089</v>
+        <v>46173</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>45998</v>
+        <v>46082</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>121</v>
@@ -3108,20 +3108,20 @@
         <v>132</v>
       </c>
       <c r="C83" s="2" t="n">
-        <v>46169</v>
+        <v>46288</v>
       </c>
       <c r="D83" s="2" t="n">
         <f aca="false">C83+4</f>
-        <v>46173</v>
+        <v>46292</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>46082</v>
+        <v>46201</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>121</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>14</v>
@@ -3135,14 +3135,14 @@
         <v>132</v>
       </c>
       <c r="C84" s="2" t="n">
-        <v>46288</v>
+        <v>46344</v>
       </c>
       <c r="D84" s="2" t="n">
         <f aca="false">C84+4</f>
-        <v>46292</v>
+        <v>46348</v>
       </c>
       <c r="E84" s="2" t="n">
-        <v>46201</v>
+        <v>46257</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>121</v>
@@ -3156,53 +3156,53 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C85" s="2" t="n">
-        <v>46344</v>
+        <v>46078</v>
       </c>
       <c r="D85" s="2" t="n">
         <f aca="false">C85+4</f>
-        <v>46348</v>
+        <v>46082</v>
       </c>
       <c r="E85" s="2" t="n">
-        <v>46257</v>
+        <v>45991</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C86" s="2" t="n">
-        <v>46078</v>
+        <v>46083</v>
       </c>
       <c r="D86" s="2" t="n">
-        <f aca="false">C86+4</f>
-        <v>46082</v>
+        <f aca="false">C86+7</f>
+        <v>46090</v>
       </c>
       <c r="E86" s="2" t="n">
-        <v>45991</v>
+        <v>45998</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>36</v>
@@ -3210,17 +3210,17 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C87" s="2" t="n">
-        <v>46083</v>
+        <v>46085</v>
       </c>
       <c r="D87" s="2" t="n">
-        <f aca="false">C87+7</f>
-        <v>46090</v>
+        <f aca="false">C87+4</f>
+        <v>46089</v>
       </c>
       <c r="E87" s="2" t="n">
         <v>45998</v>
@@ -3237,26 +3237,25 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C88" s="2" t="n">
-        <v>46085</v>
-      </c>
-      <c r="D88" s="2" t="n">
-        <f aca="false">C88+4</f>
-        <v>46089</v>
+        <v>138</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>140</v>
       </c>
       <c r="E88" s="2" t="n">
-        <v>45998</v>
+        <v>46103</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>36</v>
@@ -3264,25 +3263,26 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
+      </c>
+      <c r="C89" s="2" t="n">
+        <v>46253</v>
+      </c>
+      <c r="D89" s="2" t="n">
+        <f aca="false">C89+4</f>
+        <v>46257</v>
       </c>
       <c r="E89" s="2" t="n">
-        <v>46103</v>
+        <v>46166</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>119</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>36</v>
@@ -3290,17 +3290,16 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C90" s="2" t="n">
         <v>46253</v>
       </c>
       <c r="D90" s="2" t="n">
-        <f aca="false">C90+4</f>
-        <v>46257</v>
+        <v>46253</v>
       </c>
       <c r="E90" s="2" t="n">
         <v>46166</v>
@@ -3309,7 +3308,7 @@
         <v>119</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>36</v>
@@ -3317,25 +3316,26 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="C91" s="2" t="n">
-        <v>46253</v>
+        <v>46251</v>
       </c>
       <c r="D91" s="2" t="n">
-        <v>46253</v>
+        <f aca="false">C91+9</f>
+        <v>46260</v>
       </c>
       <c r="E91" s="2" t="n">
         <v>46166</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>36</v>
@@ -3343,30 +3343,30 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="C92" s="2" t="n">
-        <v>46251</v>
+        <v>46129</v>
       </c>
       <c r="D92" s="2" t="n">
-        <f aca="false">C92+9</f>
-        <v>46260</v>
+        <v>46138</v>
       </c>
       <c r="E92" s="2" t="n">
-        <v>46166</v>
+        <v>46089</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="J92" s="2"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
@@ -3388,7 +3388,7 @@
         <v>146</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>19</v>
@@ -3403,19 +3403,19 @@
         <v>56</v>
       </c>
       <c r="C94" s="2" t="n">
-        <v>46129</v>
+        <v>46202</v>
       </c>
       <c r="D94" s="2" t="n">
-        <v>46138</v>
+        <v>46208</v>
       </c>
       <c r="E94" s="2" t="n">
-        <v>46089</v>
+        <v>46152</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>19</v>
@@ -3430,19 +3430,19 @@
         <v>56</v>
       </c>
       <c r="C95" s="2" t="n">
-        <v>46202</v>
+        <v>46251</v>
       </c>
       <c r="D95" s="2" t="n">
-        <v>46208</v>
+        <v>46260</v>
       </c>
       <c r="E95" s="2" t="n">
-        <v>46152</v>
+        <v>46180</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>13</v>
+        <v>150</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>19</v>
@@ -3457,19 +3457,19 @@
         <v>56</v>
       </c>
       <c r="C96" s="2" t="n">
-        <v>46251</v>
+        <v>46339</v>
       </c>
       <c r="D96" s="2" t="n">
-        <v>46260</v>
+        <v>46348</v>
       </c>
       <c r="E96" s="2" t="n">
-        <v>46180</v>
+        <v>46310</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>19</v>
@@ -3478,25 +3478,25 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C97" s="2" t="n">
-        <v>46339</v>
+        <v>46325</v>
       </c>
       <c r="D97" s="2" t="n">
-        <v>46348</v>
+        <v>46334</v>
       </c>
       <c r="E97" s="2" t="n">
-        <v>46310</v>
+        <v>46278</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>19</v>
@@ -3505,25 +3505,25 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C98" s="2" t="n">
-        <v>46325</v>
+        <v>46202</v>
       </c>
       <c r="D98" s="2" t="n">
-        <v>46334</v>
+        <v>46208</v>
       </c>
       <c r="E98" s="2" t="n">
-        <v>46278</v>
+        <v>46152</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>19</v>
@@ -3538,19 +3538,19 @@
         <v>62</v>
       </c>
       <c r="C99" s="2" t="n">
-        <v>46202</v>
+        <v>46325</v>
       </c>
       <c r="D99" s="2" t="n">
-        <v>46208</v>
+        <v>46334</v>
       </c>
       <c r="E99" s="2" t="n">
-        <v>46152</v>
+        <v>46278</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>19</v>
@@ -3565,19 +3565,19 @@
         <v>62</v>
       </c>
       <c r="C100" s="2" t="n">
-        <v>46325</v>
+        <v>46349</v>
       </c>
       <c r="D100" s="2" t="n">
-        <v>46334</v>
+        <v>46358</v>
       </c>
       <c r="E100" s="2" t="n">
-        <v>46278</v>
+        <v>46307</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>19</v>
@@ -3586,10 +3586,10 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="C101" s="2" t="n">
         <v>46349</v>
@@ -3613,10 +3613,10 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C102" s="2" t="n">
         <v>46349</v>
@@ -3640,37 +3640,37 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>27</v>
+        <v>155</v>
       </c>
       <c r="C103" s="2" t="n">
-        <v>46349</v>
+        <v>46293</v>
       </c>
       <c r="D103" s="2" t="n">
-        <v>46358</v>
+        <v>46297</v>
       </c>
       <c r="E103" s="2" t="n">
-        <v>46307</v>
+        <v>46180</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J103" s="2"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C104" s="2" t="n">
         <v>46293</v>
@@ -3694,25 +3694,25 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C105" s="2" t="n">
-        <v>46293</v>
+        <v>46051</v>
       </c>
       <c r="D105" s="2" t="n">
-        <v>46297</v>
+        <v>46054</v>
       </c>
       <c r="E105" s="2" t="n">
-        <v>46180</v>
+        <v>46029</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>14</v>
@@ -3754,19 +3754,19 @@
         <v>158</v>
       </c>
       <c r="C107" s="2" t="n">
-        <v>46135</v>
+        <v>46247</v>
       </c>
       <c r="D107" s="2" t="n">
-        <v>46138</v>
+        <v>46250</v>
       </c>
       <c r="E107" s="2" t="n">
-        <v>46113</v>
+        <v>46180</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>14</v>
@@ -3781,19 +3781,19 @@
         <v>158</v>
       </c>
       <c r="C108" s="2" t="n">
-        <v>46247</v>
+        <v>46268</v>
       </c>
       <c r="D108" s="2" t="n">
-        <v>46250</v>
+        <v>46271</v>
       </c>
       <c r="E108" s="2" t="n">
-        <v>46180</v>
+        <v>46236</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
@@ -3808,13 +3808,13 @@
         <v>158</v>
       </c>
       <c r="C109" s="2" t="n">
-        <v>46268</v>
+        <v>46338</v>
       </c>
       <c r="D109" s="2" t="n">
-        <v>46271</v>
+        <v>46341</v>
       </c>
       <c r="E109" s="2" t="n">
-        <v>46236</v>
+        <v>46299</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>146</v>
@@ -3829,19 +3829,19 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>158</v>
+        <v>90</v>
       </c>
       <c r="C110" s="2" t="n">
-        <v>46338</v>
+        <v>46169</v>
       </c>
       <c r="D110" s="2" t="n">
-        <v>46341</v>
+        <v>46173</v>
       </c>
       <c r="E110" s="2" t="n">
-        <v>46299</v>
+        <v>46131</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>146</v>
@@ -3854,7 +3854,7 @@
       </c>
       <c r="J110" s="2"/>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
         <v>68</v>
       </c>
@@ -3862,13 +3862,13 @@
         <v>90</v>
       </c>
       <c r="C111" s="2" t="n">
-        <v>46169</v>
+        <v>46309</v>
       </c>
       <c r="D111" s="2" t="n">
-        <v>46173</v>
+        <v>46313</v>
       </c>
       <c r="E111" s="2" t="n">
-        <v>46131</v>
+        <v>46271</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>146</v>
@@ -3883,52 +3883,52 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="C112" s="2" t="n">
-        <v>46309</v>
+        <v>46042</v>
       </c>
       <c r="D112" s="2" t="n">
-        <v>46313</v>
+        <v>46043</v>
       </c>
       <c r="E112" s="2" t="n">
-        <v>46271</v>
+        <v>45976</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="J112" s="2"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="C113" s="2" t="n">
-        <v>46042</v>
+        <v>46069</v>
       </c>
       <c r="D113" s="2" t="n">
-        <v>46043</v>
+        <v>46072</v>
       </c>
       <c r="E113" s="2" t="n">
-        <v>45976</v>
+        <v>46040</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>149</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>13</v>
+        <v>150</v>
       </c>
       <c r="H113" s="1" t="s">
         <v>36</v>
@@ -3937,10 +3937,10 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C114" s="2" t="n">
         <v>46069</v>
@@ -3964,25 +3964,25 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="C115" s="2" t="n">
-        <v>46069</v>
+        <v>46076</v>
       </c>
       <c r="D115" s="2" t="n">
-        <v>46072</v>
+        <v>46082</v>
       </c>
       <c r="E115" s="2" t="n">
-        <v>46040</v>
+        <v>46041</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>36</v>
@@ -3997,19 +3997,19 @@
         <v>94</v>
       </c>
       <c r="C116" s="2" t="n">
-        <v>46076</v>
+        <v>46251</v>
       </c>
       <c r="D116" s="2" t="n">
-        <v>46082</v>
+        <v>46260</v>
       </c>
       <c r="E116" s="2" t="n">
-        <v>46041</v>
+        <v>46180</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>36</v>
@@ -4023,20 +4023,20 @@
       <c r="B117" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C117" s="2" t="n">
-        <v>46251</v>
-      </c>
-      <c r="D117" s="2" t="n">
-        <v>46260</v>
+      <c r="C117" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="E117" s="2" t="n">
-        <v>46180</v>
+        <v>46054</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>36</v>
@@ -4045,25 +4045,25 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>94</v>
+        <v>163</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E118" s="2" t="n">
-        <v>46054</v>
+        <v>46257</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>36</v>
@@ -4077,20 +4077,20 @@
       <c r="B119" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>165</v>
+      <c r="C119" s="2" t="n">
+        <v>46328</v>
+      </c>
+      <c r="D119" s="2" t="n">
+        <v>46337</v>
       </c>
       <c r="E119" s="2" t="n">
-        <v>46257</v>
+        <v>46271</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>13</v>
+        <v>150</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>36</v>
@@ -4105,40 +4105,40 @@
         <v>163</v>
       </c>
       <c r="C120" s="2" t="n">
-        <v>46328</v>
+        <v>46339</v>
       </c>
       <c r="D120" s="2" t="n">
-        <v>46337</v>
+        <v>46348</v>
       </c>
       <c r="E120" s="2" t="n">
-        <v>46271</v>
+        <v>46310</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J120" s="2"/>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>162</v>
+        <v>91</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C121" s="2" t="n">
-        <v>46339</v>
+        <v>46129</v>
       </c>
       <c r="D121" s="2" t="n">
-        <v>46348</v>
+        <v>46138</v>
       </c>
       <c r="E121" s="2" t="n">
-        <v>46310</v>
+        <v>46113</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>151</v>
@@ -4159,13 +4159,13 @@
         <v>166</v>
       </c>
       <c r="C122" s="2" t="n">
-        <v>46129</v>
+        <v>46339</v>
       </c>
       <c r="D122" s="2" t="n">
-        <v>46138</v>
+        <v>46348</v>
       </c>
       <c r="E122" s="2" t="n">
-        <v>46113</v>
+        <v>46310</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>151</v>
@@ -4186,40 +4186,42 @@
         <v>166</v>
       </c>
       <c r="C123" s="2" t="n">
-        <v>46339</v>
+        <v>46137</v>
       </c>
       <c r="D123" s="2" t="n">
-        <v>46348</v>
+        <v>46138</v>
       </c>
       <c r="E123" s="2" t="n">
-        <v>46310</v>
+        <v>46103</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>152</v>
+        <v>13</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J123" s="2"/>
+      <c r="J123" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C124" s="2" t="n">
-        <v>46137</v>
+        <v>46314</v>
       </c>
       <c r="D124" s="2" t="n">
-        <v>46138</v>
+        <v>46318</v>
       </c>
       <c r="E124" s="2" t="n">
-        <v>46103</v>
+        <v>46285</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>148</v>
@@ -4230,66 +4232,37 @@
       <c r="H124" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J124" s="2" t="s">
-        <v>167</v>
-      </c>
+      <c r="J124" s="2"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C125" s="2" t="n">
-        <v>46314</v>
+        <v>46342</v>
       </c>
       <c r="D125" s="2" t="n">
-        <v>46318</v>
+        <v>46348</v>
       </c>
       <c r="E125" s="2" t="n">
-        <v>46285</v>
+        <v>46306</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="J125" s="2"/>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C126" s="2" t="n">
-        <v>46342</v>
-      </c>
-      <c r="D126" s="2" t="n">
-        <v>46348</v>
-      </c>
-      <c r="E126" s="2" t="n">
-        <v>46306</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H126" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J126" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J126"/>
+  <autoFilter ref="A1:J125"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>